<commit_message>
Add password for Create-account feature
</commit_message>
<xml_diff>
--- a/player.xlsx
+++ b/player.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -423,6 +423,7 @@
     <col width="16.46484375" customWidth="1" min="1" max="1"/>
     <col width="24.6640625" customWidth="1" min="2" max="2"/>
     <col width="26.265625" customWidth="1" min="3" max="3"/>
+    <col width="13.19921875" customWidth="1" min="4" max="4"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -443,10 +444,15 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>password</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>coin</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>char_class</t>
         </is>
@@ -466,6 +472,28 @@
       <c r="C2" t="inlineStr">
         <is>
           <t>Loc.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Loc Le</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ltloc05lumia520@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Loc Le.png</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>khongbiethehe</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Change Background Music && Add Login feature
</commit_message>
<xml_diff>
--- a/player.xlsx
+++ b/player.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -447,10 +447,8 @@
           <t>password</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>coin</t>
-        </is>
+      <c r="E1" t="n">
+        <v>0</v>
       </c>
       <c r="F1" t="inlineStr">
         <is>
@@ -461,7 +459,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Loc</t>
+          <t>Loc Le</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -471,30 +469,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Loc.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Loc Le</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>ltloc05lumia520@gmail.com</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
           <t>Loc Le.png</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>khongbiethehe</t>
         </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Face recognition in Login
</commit_message>
<xml_diff>
--- a/player.xlsx
+++ b/player.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -459,26 +459,26 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Loc Le</t>
+          <t>Loc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ltloc05lumia520@gmail.com</t>
+          <t>fff</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Loc Le.png</t>
+          <t>Loc.png</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>khongbiethehe</t>
+          <t>ff</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>24</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in processing data from database
</commit_message>
<xml_diff>
--- a/player.xlsx
+++ b/player.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -447,8 +447,10 @@
           <t>password</t>
         </is>
       </c>
-      <c r="E1" t="n">
-        <v>0</v>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>coin</t>
+        </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
@@ -478,7 +480,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>